<commit_message>
DB connection and Retry logic
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Automation/AbekaTemp/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5064547D-C43F-2D43-8040-B3A2F64E8A4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706B812A-E8C0-7244-8437-939CCFCACE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="9380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>rcg@pcci.edu</t>
   </si>
@@ -41,15 +41,28 @@
   </si>
   <si>
     <t>syed.rcg</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>Hello, RCG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -82,11 +95,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,32 +382,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -406,7 +426,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50012846-BBBE-8F49-8572-8B537A72021A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -414,15 +434,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Allure fix and Digital assessment new query implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Automation/AbekaTemp/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68BB131-1A7D-EF4C-A6C4-8AEF49989CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCFB5E0-16ED-E149-A04C-66E07BE1F0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParentCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="StudentCredentials" sheetId="2" r:id="rId2"/>
+    <sheet name="GradeOneStudentCredentials" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>rcg@pcci.edu</t>
   </si>
@@ -53,6 +54,21 @@
   </si>
   <si>
     <t>RCG Testing</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>AutoGoHlE_208</t>
+  </si>
+  <si>
+    <t>AutoVPGad_263</t>
+  </si>
+  <si>
+    <t>AutoglwqZ_839</t>
+  </si>
+  <si>
+    <t>AutoiEIjf_985</t>
   </si>
 </sst>
 </file>
@@ -390,14 +406,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -441,10 +458,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -466,6 +489,69 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903AAD5F-E2CA-8F41-81A5-DCE49C6E583F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enrollment 4 and 9
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -3,23 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Automation/AbekaTemp/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCFB5E0-16ED-E149-A04C-66E07BE1F0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C153E6-E2A9-6641-BA71-D7D9E158640C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParentCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="StudentCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="GradeOneStudentCredentials" sheetId="3" r:id="rId3"/>
+    <sheet name="Grade4StudentCredentials" sheetId="4" r:id="rId4"/>
+    <sheet name="Grade9StudentCredentials" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>rcg@pcci.edu</t>
   </si>
@@ -69,13 +71,23 @@
   </si>
   <si>
     <t>AutoiEIjf_985</t>
+  </si>
+  <si>
+    <t>Auto2021_07_16_01_25_46_129</t>
+  </si>
+  <si>
+    <t>Auto2021_07_16_01_33_33_468</t>
+  </si>
+  <si>
+    <t>Auto20210719181533106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,9 +424,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -463,10 +475,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -501,14 +513,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903AAD5F-E2CA-8F41-81A5-DCE49C6E583F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -558,4 +570,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F814710-126C-F845-8A8F-5D817919A993}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.5" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D1542F-B48A-6941-87AE-0D73394C5070}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.13671875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create account api and graduate petition
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>rcg@pcci.edu</t>
   </si>
@@ -81,13 +81,17 @@
   </si>
   <si>
     <t>Auto20210719181533106</t>
+  </si>
+  <si>
+    <t>Auto20210827004426713</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,9 +428,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -476,10 +480,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -520,8 +524,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -583,7 +587,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.5" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -631,7 +635,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.1640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -670,6 +674,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.13671875" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -685,6 +692,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented excel data in Digital assessment TC
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E02E7FC-A28F-8446-BDA2-F74E5E225140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358ADA4B-7044-B348-844B-41B338991B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParentCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="StudentCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="GradeWiseVideoList" sheetId="7" r:id="rId3"/>
     <sheet name="GradeOneVideoList" sheetId="4" r:id="rId4"/>
-    <sheet name="DigitalAssessmentList" sheetId="3" r:id="rId5"/>
-    <sheet name="Grade9StudentCredentials" sheetId="5" r:id="rId6"/>
+    <sheet name="GradeNineVideoList" sheetId="5" r:id="rId5"/>
+    <sheet name="DigitalAssessmentList" sheetId="3" r:id="rId6"/>
     <sheet name="Grade12StudentCredentials" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="76">
   <si>
     <t>Password</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Password@123</t>
   </si>
   <si>
-    <t>Auto20210719181533106</t>
-  </si>
-  <si>
     <t>Auto20210827004426713</t>
   </si>
   <si>
@@ -90,24 +87,12 @@
     <t>Grade 12</t>
   </si>
   <si>
-    <t>ATM202110281531</t>
-  </si>
-  <si>
-    <t>ATM202110281531 ATM202110281531</t>
-  </si>
-  <si>
     <t>ATM202110281958</t>
   </si>
   <si>
     <t>ATM202110281958 ATM202110281958</t>
   </si>
   <si>
-    <t>ATM202110290054</t>
-  </si>
-  <si>
-    <t>ATM202110290054 ATM202110290054</t>
-  </si>
-  <si>
     <t>Bible</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>Hebrew History</t>
   </si>
   <si>
-    <t>English 9</t>
-  </si>
-  <si>
     <t>Algebra 1</t>
   </si>
   <si>
@@ -186,39 +168,6 @@
     <t>Health</t>
   </si>
   <si>
-    <t>Content Quiz 4</t>
-  </si>
-  <si>
-    <t>Speed/Comprehension Quiz 6</t>
-  </si>
-  <si>
-    <t>Grammar Quiz 7</t>
-  </si>
-  <si>
-    <t>Quiz 12</t>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="15"/>
-        <color rgb="FF444444"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Appendix Quiz F</t>
-    </r>
-  </si>
-  <si>
-    <t>Quiz 11</t>
-  </si>
-  <si>
-    <t>Quiz 9</t>
-  </si>
-  <si>
     <t>SegmentId</t>
   </si>
   <si>
@@ -261,12 +210,6 @@
     <t>27584641</t>
   </si>
   <si>
-    <t>rcg+27584642@pcci.edu</t>
-  </si>
-  <si>
-    <t>rcg27584642</t>
-  </si>
-  <si>
     <t>27584642</t>
   </si>
   <si>
@@ -304,13 +247,25 @@
   </si>
   <si>
     <t>FirstgradeIT1</t>
+  </si>
+  <si>
+    <t>Content Quiz 1</t>
+  </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t>Appendix Quiz A</t>
+  </si>
+  <si>
+    <t>NinthgradeIT1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,13 +307,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="15"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9.8000000000000007"/>
@@ -418,8 +366,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -706,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -729,18 +677,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3">
         <v>27583950</v>
@@ -748,64 +696,64 @@
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{10CF41B5-1ECE-C740-B375-B40D4BD2B945}"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="mailto:ABATestAccount@pcci.edu" display="mailto:ABATestAccount@pcci.edu" xr:uid="{CBB1F535-7EFB-D349-AB45-8B58256234AE}"/>
+    <hyperlink ref="A3" r:id="rId1" tooltip="mailto:ABATestAccount@pcci.edu" display="mailto:ABATestAccount@pcci.edu" xr:uid="{CBB1F535-7EFB-D349-AB45-8B58256234AE}"/>
+    <hyperlink ref="A6" r:id="rId2" tooltip="mailto:ABATestAccount@pcci.edu" display="mailto:ABATestAccount@pcci.edu" xr:uid="{172ED60C-25B4-D54C-B33E-5F5EBA95D3CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -820,7 +768,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -839,80 +787,80 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -939,39 +887,39 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2">
@@ -983,16 +931,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3">
@@ -1004,16 +952,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4">
@@ -1025,16 +973,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5">
@@ -1046,16 +994,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6">
@@ -1067,16 +1015,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7">
@@ -1088,16 +1036,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8">
@@ -1109,10 +1057,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="C9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9">
@@ -1124,10 +1072,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="C10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10">
@@ -1148,7 +1096,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1158,39 +1106,39 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2">
@@ -1202,16 +1150,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3">
@@ -1223,16 +1171,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4">
@@ -1244,16 +1192,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5">
@@ -1265,16 +1213,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6">
@@ -1286,16 +1234,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7">
@@ -1307,16 +1255,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8">
@@ -1328,13 +1276,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9">
@@ -1346,13 +1294,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10">
@@ -1368,11 +1316,179 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D1542F-B48A-6941-87AE-0D73394C5070}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903AAD5F-E2CA-8F41-81A5-DCE49C6E583F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1384,24 +1500,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16">
       <c r="A1" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10" t="b">
@@ -1410,10 +1526,10 @@
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="b">
@@ -1422,10 +1538,10 @@
     </row>
     <row r="4" spans="1:4" ht="16">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="b">
@@ -1434,92 +1550,31 @@
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="19">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D1542F-B48A-6941-87AE-0D73394C5070}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1549,7 +1604,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
ABA hold removal logic implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="145">
   <si>
     <t>Password</t>
   </si>
@@ -386,6 +386,87 @@
   </si>
   <si>
     <t>ATM202111222327 ATM202111222327</t>
+  </si>
+  <si>
+    <t>rcg+27584685@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584685</t>
+  </si>
+  <si>
+    <t>27584685</t>
+  </si>
+  <si>
+    <t>ATM202111251820</t>
+  </si>
+  <si>
+    <t>ATM202111251820 ATM202111251820</t>
+  </si>
+  <si>
+    <t>rcg+27584686@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584686</t>
+  </si>
+  <si>
+    <t>27584686</t>
+  </si>
+  <si>
+    <t>rcg+27584687@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584687</t>
+  </si>
+  <si>
+    <t>27584687</t>
+  </si>
+  <si>
+    <t>rcg+27584688@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584688</t>
+  </si>
+  <si>
+    <t>27584688</t>
+  </si>
+  <si>
+    <t>rcg+27584689@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584689</t>
+  </si>
+  <si>
+    <t>27584689</t>
+  </si>
+  <si>
+    <t>ATM202111251944</t>
+  </si>
+  <si>
+    <t>ATM202111251944 ATM202111251944</t>
+  </si>
+  <si>
+    <t>rcg+27584690@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584690</t>
+  </si>
+  <si>
+    <t>27584690</t>
+  </si>
+  <si>
+    <t>ATM202111251958</t>
+  </si>
+  <si>
+    <t>ATM202111251958 ATM202111251958</t>
+  </si>
+  <si>
+    <t>rcg+27584691@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27584691</t>
+  </si>
+  <si>
+    <t>27584691</t>
   </si>
 </sst>
 </file>
@@ -947,7 +1028,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.80078125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.75" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="32.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
@@ -983,58 +1064,58 @@
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" s="9" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1096,13 +1177,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1110,13 +1191,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1124,13 +1205,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>

</xml_diff>